<commit_message>
diagram and assessment results
</commit_message>
<xml_diff>
--- a/static/assessment-results.xlsx
+++ b/static/assessment-results.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Desktop\projects\ssa-200\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8ECED2-3717-4E17-8771-A944A65FD74D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4CBA6B-24F1-45C8-A55B-B9621D681191}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" activeTab="1" xr2:uid="{13FE1660-FF3F-4AAD-AD17-F58810B5493C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" xr2:uid="{13FE1660-FF3F-4AAD-AD17-F58810B5493C}"/>
   </bookViews>
   <sheets>
-    <sheet name="qs" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
-    <sheet name="responses" sheetId="1" r:id="rId3"/>
-    <sheet name="scores" sheetId="4" r:id="rId4"/>
+    <sheet name="responses - la" sheetId="7" r:id="rId1"/>
+    <sheet name="qs" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="responses" sheetId="1" r:id="rId4"/>
+    <sheet name="scores" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
-    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,6 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="24">
   <si>
     <t>question</t>
   </si>
@@ -116,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -154,7 +156,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4118,7 +4120,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4FDADDD3-E0A2-40D8-BD0B-937A4185D9C9}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4FDADDD3-E0A2-40D8-BD0B-937A4185D9C9}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4215,7 +4217,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F2085C4-EB59-4978-A478-5165FFB6D1A1}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F2085C4-EB59-4978-A478-5165FFB6D1A1}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -4756,6 +4758,2081 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9857842E-A391-4466-B7DE-A67FA43B9491}">
+  <dimension ref="A1:F133"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65:D133"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>IF(C2="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>IF(E2="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f>IF(C3="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>IF(E3="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f>IF(C4="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>IF(E4="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <f>IF(C5="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>IF(E5="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f>IF(C6="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>IF(E6="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>IF(C7="a",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>IF(E7="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f>IF(C8="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>IF(E8="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f>IF(C9="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>IF(E9="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>IF(C10="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>IF(E10="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <f>IF(C11="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>IF(E11="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f>IF(C12="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>IF(E12="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f>IF(C13="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f>IF(E13="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f>IF(C14="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>IF(E14="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>IF(C15="a",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f>IF(E15="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <f>IF(C16="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f>IF(E16="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f>IF(C17="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>IF(E17="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f>IF(C18="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f>IF(E18="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <f>IF(C19="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>IF(E19="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <f>IF(C20="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>IF(E20="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f>IF(C21="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f>IF(E21="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f>IF(C22="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f>IF(E22="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>IF(C23="a",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f>IF(E23="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <f>IF(C24="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f>IF(E24="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f>IF(C25="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f>IF(E25="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f>IF(C26="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f>IF(E26="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <f>IF(C27="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>IF(E27="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <f>IF(C28="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>IF(E28="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <f>IF(C29="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f>IF(E29="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <f>IF(C30="c",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f>IF(E30="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>IF(C31="a",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f>IF(E31="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <f>IF(C32="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f>IF(E32="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f>IF(C33="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <f>IF(E33="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <f>IF(C34="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f>IF(E34="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <f>IF(C35="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f>IF(E35="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <f>IF(C36="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <f>IF(E36="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <f>IF(C37="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <f>IF(E37="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <f>IF(C38="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <f>IF(E38="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <f>IF(C39="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>IF(E39="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <f>IF(C40="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>IF(E40="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <f>IF(C41="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f>IF(E41="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <f>IF(C42="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f>IF(E42="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>11</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <f>IF(C43="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f>IF(E43="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <f>IF(C44="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <f>IF(E44="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <f>IF(C45="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <f>IF(E45="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <f>IF(C46="c",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <f>IF(E46="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <f>IF(C47="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <f>IF(E47="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <f>IF(C48="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <f>IF(E48="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <f>IF(C49="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <f>IF(E49="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <f>IF(C50="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <f>IF(E50="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <f>IF(C51="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f>IF(E51="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>13</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <f>IF(C52="b",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <f>IF(E52="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <f>IF(C53="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <f>IF(E53="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <f>IF(C54="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <f>IF(E54="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>14</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <f>IF(C55="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f>IF(E55="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <f>IF(C56="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <f>IF(E56="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>14</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <f>IF(C57="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <f>IF(E57="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>15</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <f>IF(C58="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <f>IF(E58="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <f>IF(C59="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f>IF(E59="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>15</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <f>IF(C60="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f>IF(E60="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>15</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <f>IF(C61="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <f>IF(E61="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <f>IF(C62="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <f>IF(E62="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>16</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <f>IF(C63="a",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <f>IF(E63="a",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>16</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <f>IF(C64="b",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <f>IF(E64="b",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <f>IF(C65="c",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <f>IF(E65="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D129" si="0">IF(C66="c",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>3</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>3</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>4</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>4</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="C108" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>3</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>3</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>4</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>3</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>4</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>3</v>
+      </c>
+      <c r="C124" t="s">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>4</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>3</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>3</v>
+      </c>
+      <c r="C128" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130">
+        <f t="shared" ref="D130:D133" si="1">IF(C130="c",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F65">
+    <sortCondition ref="A2:A65"/>
+    <sortCondition ref="B2:B65"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6282C17B-192D-4BC5-BC5A-5394C5306C3B}">
   <dimension ref="A3:C9"/>
   <sheetViews>
@@ -4851,11 +6928,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D617A9D1-57A2-4464-A51A-7BE358750B24}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -5162,12 +7239,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BAC29A-10FC-4162-9923-7B812E7DB352}">
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5206,7 +7283,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <f>IF(C2="c",1,0)</f>
+        <f t="shared" ref="D2:D17" si="0">IF(C2="c",1,0)</f>
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -5228,14 +7305,14 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f>IF(C3="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="0">IF(E3="c",1,0)</f>
+        <f t="shared" ref="F3:F17" si="1">IF(E3="c",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -5250,14 +7327,14 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f>IF(C4="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5272,14 +7349,14 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <f>IF(C5="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5294,14 +7371,14 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <f>IF(C6="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5316,14 +7393,14 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <f>IF(C7="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5338,14 +7415,14 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <f>IF(C8="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5360,14 +7437,14 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <f>IF(C9="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5382,14 +7459,14 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <f>IF(C10="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5404,14 +7481,14 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <f>IF(C11="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5426,14 +7503,14 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <f>IF(C12="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5448,14 +7525,14 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <f>IF(C13="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5470,14 +7547,14 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <f>IF(C14="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5492,14 +7569,14 @@
         <v>5</v>
       </c>
       <c r="D15">
-        <f>IF(C15="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5514,14 +7591,14 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <f>IF(C16="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5536,14 +7613,14 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <f>IF(C17="c",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5558,7 +7635,7 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <f>IF(C18="a",1,0)</f>
+        <f t="shared" ref="D18:D33" si="2">IF(C18="a",1,0)</f>
         <v>0</v>
       </c>
       <c r="E18" t="s">
@@ -5580,14 +7657,14 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <f>IF(C19="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F33" si="1">IF(E19="a",1,0)</f>
+        <f t="shared" ref="F19:F33" si="3">IF(E19="a",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -5602,14 +7679,14 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <f>IF(C20="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5624,14 +7701,14 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <f>IF(C21="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5646,14 +7723,14 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f>IF(C22="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5668,14 +7745,14 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <f>IF(C23="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5690,14 +7767,14 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <f>IF(C24="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5712,14 +7789,14 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <f>IF(C25="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5734,14 +7811,14 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <f>IF(C26="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5756,14 +7833,14 @@
         <v>5</v>
       </c>
       <c r="D27">
-        <f>IF(C27="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5778,14 +7855,14 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <f>IF(C28="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5800,14 +7877,14 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <f>IF(C29="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5822,14 +7899,14 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <f>IF(C30="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5844,14 +7921,14 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <f>IF(C31="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5866,14 +7943,14 @@
         <v>5</v>
       </c>
       <c r="D32">
-        <f>IF(C32="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5888,14 +7965,14 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <f>IF(C33="a",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5910,7 +7987,7 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <f>IF(C34="b",1,0)</f>
+        <f t="shared" ref="D34:D49" si="4">IF(C34="b",1,0)</f>
         <v>0</v>
       </c>
       <c r="E34" t="s">
@@ -5932,14 +8009,14 @@
         <v>3</v>
       </c>
       <c r="D35">
-        <f>IF(C35="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E35" t="s">
         <v>3</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F49" si="2">IF(E35="b",1,0)</f>
+        <f t="shared" ref="F35:F49" si="5">IF(E35="b",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -5954,14 +8031,14 @@
         <v>3</v>
       </c>
       <c r="D36">
-        <f>IF(C36="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>6</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5976,14 +8053,14 @@
         <v>5</v>
       </c>
       <c r="D37">
-        <f>IF(C37="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5998,14 +8075,14 @@
         <v>5</v>
       </c>
       <c r="D38">
-        <f>IF(C38="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E38" t="s">
         <v>1</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6020,14 +8097,14 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <f>IF(C39="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E39" t="s">
         <v>2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6042,14 +8119,14 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <f>IF(C40="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6064,14 +8141,14 @@
         <v>5</v>
       </c>
       <c r="D41">
-        <f>IF(C41="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6086,14 +8163,14 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <f>IF(C42="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6108,14 +8185,14 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <f>IF(C43="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6130,14 +8207,14 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <f>IF(C44="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E44" t="s">
         <v>5</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6152,14 +8229,14 @@
         <v>1</v>
       </c>
       <c r="D45">
-        <f>IF(C45="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6174,14 +8251,14 @@
         <v>5</v>
       </c>
       <c r="D46">
-        <f>IF(C46="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6196,14 +8273,14 @@
         <v>6</v>
       </c>
       <c r="D47">
-        <f>IF(C47="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6218,14 +8295,14 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <f>IF(C48="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -6240,14 +8317,14 @@
         <v>5</v>
       </c>
       <c r="D49">
-        <f>IF(C49="b",1,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -6262,7 +8339,7 @@
         <v>1</v>
       </c>
       <c r="D50">
-        <f>IF(C50="c",1,0)</f>
+        <f t="shared" ref="D50:D65" si="6">IF(C50="c",1,0)</f>
         <v>0</v>
       </c>
       <c r="E50" t="s">
@@ -6284,14 +8361,14 @@
         <v>2</v>
       </c>
       <c r="D51">
-        <f>IF(C51="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E51" t="s">
         <v>2</v>
       </c>
       <c r="F51">
-        <f t="shared" ref="F51:F65" si="3">IF(E51="c",1,0)</f>
+        <f t="shared" ref="F51:F65" si="7">IF(E51="c",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -6306,14 +8383,14 @@
         <v>5</v>
       </c>
       <c r="D52">
-        <f>IF(C52="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E52" t="s">
         <v>2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6328,14 +8405,14 @@
         <v>2</v>
       </c>
       <c r="D53">
-        <f>IF(C53="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
       </c>
       <c r="F53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6350,14 +8427,14 @@
         <v>2</v>
       </c>
       <c r="D54">
-        <f>IF(C54="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6372,14 +8449,14 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <f>IF(C55="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E55" t="s">
         <v>1</v>
       </c>
       <c r="F55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6394,14 +8471,14 @@
         <v>2</v>
       </c>
       <c r="D56">
-        <f>IF(C56="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
       </c>
       <c r="F56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6416,14 +8493,14 @@
         <v>5</v>
       </c>
       <c r="D57">
-        <f>IF(C57="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6438,14 +8515,14 @@
         <v>2</v>
       </c>
       <c r="D58">
-        <f>IF(C58="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E58" t="s">
         <v>2</v>
       </c>
       <c r="F58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6460,14 +8537,14 @@
         <v>1</v>
       </c>
       <c r="D59">
-        <f>IF(C59="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
       </c>
       <c r="F59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6482,14 +8559,14 @@
         <v>2</v>
       </c>
       <c r="D60">
-        <f>IF(C60="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6504,14 +8581,14 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <f>IF(C61="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6526,14 +8603,14 @@
         <v>2</v>
       </c>
       <c r="D62">
-        <f>IF(C62="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
       </c>
       <c r="F62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6548,14 +8625,14 @@
         <v>2</v>
       </c>
       <c r="D63">
-        <f>IF(C63="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E63" t="s">
         <v>2</v>
       </c>
       <c r="F63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6570,14 +8647,14 @@
         <v>5</v>
       </c>
       <c r="D64">
-        <f>IF(C64="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E64" t="s">
         <v>2</v>
       </c>
       <c r="F64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -6592,26 +8669,26 @@
         <v>2</v>
       </c>
       <c r="D65">
-        <f>IF(C65="c",1,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E65" t="s">
         <v>5</v>
       </c>
       <c r="F65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F66">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F66">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E57421-6A88-47D8-AEAF-9CD0E08B5C12}">
   <dimension ref="A3:I22"/>
   <sheetViews>

</xml_diff>